<commit_message>
Added crossover, mutation, logging & exit conditions
</commit_message>
<xml_diff>
--- a/Magic Square/Workbook.xlsx
+++ b/Magic Square/Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callu\Documents\Study\HackerRank\Magic Square\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9AA174-40FF-4233-8A52-039F24E670AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A455161F-6755-4FF2-8129-C71E8E3BAEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26085" yWindow="3090" windowWidth="21600" windowHeight="11100" xr2:uid="{BF84A0E7-C787-466B-84A6-9C6B3CD38009}"/>
+    <workbookView xWindow="1155" yWindow="2505" windowWidth="21600" windowHeight="11100" xr2:uid="{BF84A0E7-C787-466B-84A6-9C6B3CD38009}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
   <si>
     <t>column</t>
   </si>
@@ -452,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,12 +552,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -978,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4129BD6B-3B7F-431A-A917-19F89FB650CA}">
-  <dimension ref="B2:V52"/>
+  <dimension ref="B2:AE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,15 +1036,17 @@
     <col min="12" max="12" width="9.140625" customWidth="1"/>
     <col min="15" max="19" width="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3" customWidth="1"/>
+    <col min="24" max="28" width="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L2" s="33" t="s">
         <v>31</v>
       </c>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1030,7 +1075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>0</v>
       </c>
@@ -1059,7 +1104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <v>1</v>
       </c>
@@ -1081,7 +1126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <v>2</v>
       </c>
@@ -1109,960 +1154,1203 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
+    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+    </row>
+    <row r="9" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="L8" s="33" t="s">
+      <c r="E9" s="1"/>
+      <c r="L9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="33"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="U8" s="33" t="s">
+      <c r="M9" s="33"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="U9" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="V8" s="33"/>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
-        <v>0</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0</v>
-      </c>
-      <c r="D9" s="9">
-        <f>ABS(B9-(3-1))</f>
-        <v>2</v>
-      </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="22">
-        <v>3</v>
-      </c>
-      <c r="H9" s="23">
-        <v>0</v>
-      </c>
-      <c r="I9" s="24">
-        <v>0</v>
-      </c>
-      <c r="J9" s="20">
-        <f>$G$3+G9+$H$3+H9+$I$3+I9</f>
-        <v>15</v>
-      </c>
-      <c r="L9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9">
-        <f>IF(J9=15,1,0) + IF(J10=15,1,0) + IF(J11=15,1,0)+ IF(J12=15,1,0)+ IF(I12=15,1,0) + IF(H12=15,1,0) + IF(G12=15,1,0) + IF(F12=15,1,0)</f>
-        <v>8</v>
-      </c>
-      <c r="O9" s="20"/>
-      <c r="P9" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="23">
-        <v>2</v>
-      </c>
-      <c r="R9" s="24">
-        <v>1</v>
-      </c>
-      <c r="S9" s="20">
-        <f>$G$3+P9+$H$3+Q9+$I$3+R9</f>
-        <v>15</v>
-      </c>
-      <c r="U9" t="s">
-        <v>27</v>
-      </c>
-      <c r="V9">
-        <f>IF(S9=15,1,0) + IF(S10=15,1,0) + IF(S11=15,1,0)+ IF(S12=15,1,0)+ IF(R12=15,1,0) + IF(Q12=15,1,0) + IF(P12=15,1,0) + IF(O12=15,1,0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="V9" s="33"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AD9" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE9" s="33"/>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>0</v>
       </c>
       <c r="C10" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" ref="D10:D17" si="0">ABS(B10-(3-1))</f>
+        <f>ABS(B10-(3-1))</f>
         <v>2</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="25">
-        <v>0</v>
-      </c>
-      <c r="H10" s="26">
-        <v>0</v>
-      </c>
-      <c r="I10" s="27">
-        <v>1</v>
+      <c r="G10" s="22">
+        <v>3</v>
+      </c>
+      <c r="H10" s="23">
+        <v>0</v>
+      </c>
+      <c r="I10" s="24">
+        <v>0</v>
       </c>
       <c r="J10" s="20">
-        <f>$G$4+G10+$H$4+H10+$I$4+I10</f>
+        <f>$G$3+G10+$H$3+H10+$I$3+I10</f>
         <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="M10">
-        <f>8-M9</f>
-        <v>0</v>
+        <f>IF(J10=15,1,0) + IF(J11=15,1,0) + IF(J12=15,1,0)+ IF(J13=15,1,0)+ IF(I13=15,1,0) + IF(H13=15,1,0) + IF(G13=15,1,0) + IF(F13=15,1,0)</f>
+        <v>8</v>
       </c>
       <c r="O10" s="20"/>
-      <c r="P10" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="26">
-        <v>0</v>
-      </c>
-      <c r="R10" s="27">
-        <v>-3</v>
+      <c r="P10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>2</v>
+      </c>
+      <c r="R10" s="24">
+        <v>1</v>
       </c>
       <c r="S10" s="20">
-        <f>$G$4+P10+$H$4+Q10+$I$4+R10</f>
+        <f>$G$3+P10+$H$3+Q10+$I$3+R10</f>
         <v>15</v>
       </c>
       <c r="U10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="V10">
-        <f>8-V9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10">
-        <v>0</v>
-      </c>
-      <c r="C11" s="11">
-        <v>2</v>
+        <f>IF(S10=15,1,0) + IF(S11=15,1,0) + IF(S12=15,1,0)+ IF(S13=15,1,0)+ IF(R13=15,1,0) + IF(Q13=15,1,0) + IF(P13=15,1,0) + IF(O13=15,1,0)</f>
+        <v>8</v>
+      </c>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="23">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="24">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="20">
+        <f>$G$3+Y10+$H$3+Z10+$I$3+AA10</f>
+        <v>15</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE10">
+        <f>IF(AB10=15,1,0) + IF(AB11=15,1,0) + IF(AB12=15,1,0)+ IF(AB13=15,1,0)+ IF(AA13=15,1,0) + IF(Z13=15,1,0) + IF(Y13=15,1,0) + IF(X13=15,1,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D11:D18" si="0">ABS(B11-(3-1))</f>
         <v>2</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="28">
-        <v>0</v>
-      </c>
-      <c r="H11" s="29">
+      <c r="G11" s="25">
+        <v>0</v>
+      </c>
+      <c r="H11" s="26">
+        <v>0</v>
+      </c>
+      <c r="I11" s="27">
+        <v>1</v>
+      </c>
+      <c r="J11" s="20">
+        <f>$G$4+G11+$H$4+H11+$I$4+I11</f>
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11">
+        <f>8-M10</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>0</v>
+      </c>
+      <c r="R11" s="27">
+        <v>-3</v>
+      </c>
+      <c r="S11" s="20">
+        <f>$G$4+P11+$H$4+Q11+$I$4+R11</f>
+        <v>15</v>
+      </c>
+      <c r="U11" t="s">
+        <v>21</v>
+      </c>
+      <c r="V11">
+        <f>8-V10</f>
+        <v>0</v>
+      </c>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="25">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="26">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="27">
+        <v>-3</v>
+      </c>
+      <c r="AB11" s="20">
+        <f>$G$4+Y11+$H$4+Z11+$I$4+AA11</f>
+        <v>15</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE11">
+        <f>8-AE10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="28">
+        <v>0</v>
+      </c>
+      <c r="H12" s="29">
         <v>3</v>
       </c>
-      <c r="I11" s="30">
-        <v>0</v>
-      </c>
-      <c r="J11" s="20">
-        <f>$G$5+G11+$H$5+H11+$I$5+I11</f>
-        <v>15</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="I12" s="30">
+        <v>0</v>
+      </c>
+      <c r="J12" s="20">
+        <f>$G$5+G12+$H$5+H12+$I$5+I12</f>
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="M11">
-        <f>ABS(G9)+ABS(H9)+ABS(I9)+ABS(G10)+ABS(H10)+ABS(I10)+ABS(G11)+ABS(H11)+ABS(I11)</f>
+      <c r="M12">
+        <f>ABS(G10)+ABS(H10)+ABS(I10)+ABS(G11)+ABS(H11)+ABS(I11)+ABS(G12)+ABS(H12)+ABS(I12)</f>
         <v>7</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="28">
+      <c r="O12" s="20"/>
+      <c r="P12" s="28">
         <v>-1</v>
       </c>
-      <c r="Q11" s="29">
-        <v>1</v>
-      </c>
-      <c r="R11" s="30">
+      <c r="Q12" s="29">
+        <v>1</v>
+      </c>
+      <c r="R12" s="30">
         <v>3</v>
       </c>
-      <c r="S11" s="20">
-        <f>$G$5+P11+$H$5+Q11+$I$5+R11</f>
-        <v>15</v>
-      </c>
-      <c r="U11" t="s">
+      <c r="S12" s="20">
+        <f>$G$5+P12+$H$5+Q12+$I$5+R12</f>
+        <v>15</v>
+      </c>
+      <c r="U12" t="s">
         <v>22</v>
       </c>
-      <c r="V11">
-        <f>ABS(P9)+ABS(Q9)+ABS(R9)+ABS(P10)+ABS(Q10)+ABS(R10)+ABS(P11)+ABS(Q11)+ABS(R11)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
-      <c r="C12" s="9">
-        <v>0</v>
-      </c>
-      <c r="D12" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E12" s="21"/>
-      <c r="F12" s="20">
-        <f>G11+H10+I9+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="G12" s="20">
-        <f>$G$3+G9+$G$4+G10+$G$5+G11</f>
-        <v>15</v>
-      </c>
-      <c r="H12" s="20">
-        <f>H11+$H$5+H10+$H$4+H9+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="I12" s="20">
-        <f>I11+$I$5+I10+$I$4+I9+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="J12" s="20">
-        <f>$G$3+G9+$H$4+H10+$I$5+I11</f>
-        <v>15</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="V12">
+        <f>ABS(P10)+ABS(Q10)+ABS(R10)+ABS(P11)+ABS(Q11)+ABS(R11)+ABS(P12)+ABS(Q12)+ABS(R12)</f>
+        <v>15</v>
+      </c>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="28">
+        <v>-1</v>
+      </c>
+      <c r="Z12" s="29">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="30">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="20">
+        <f>$G$5+Y12+$H$5+Z12+$I$5+AA12</f>
+        <v>15</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE12">
+        <f>ABS(Y10)+ABS(Z10)+ABS(AA10)+ABS(Y11)+ABS(Z11)+ABS(AA11)+ABS(Y12)+ABS(Z12)+ABS(AA12)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20">
+        <f>G12+H11+I10+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="G13" s="20">
+        <f>$G$3+G10+$G$4+G11+$G$5+G12</f>
+        <v>15</v>
+      </c>
+      <c r="H13" s="20">
+        <f>H12+$H$5+H11+$H$4+H10+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="I13" s="20">
+        <f>I12+$I$5+I11+$I$4+I10+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="J13" s="20">
+        <f>$G$3+G10+$H$4+H11+$I$5+I12</f>
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
         <v>28</v>
       </c>
-      <c r="M12">
-        <f>((M10)+1)^2</f>
-        <v>1</v>
-      </c>
-      <c r="O12" s="20">
-        <f>P11+Q10+R9+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="P12" s="20">
-        <f>$G$3+P9+$G$4+P10+$G$5+P11</f>
-        <v>15</v>
-      </c>
-      <c r="Q12" s="20">
-        <f>Q11+$H$5+Q10+$H$4+Q9+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="R12" s="20">
-        <f>R11+$I$5+R10+$I$4+R9+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="S12" s="20">
-        <f>$G$3+P9+$H$4+Q10+$I$5+R11</f>
-        <v>15</v>
-      </c>
-      <c r="U12" t="s">
+      <c r="M13">
+        <f>((M11)+1)^2</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="20">
+        <f>P12+Q11+R10+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="P13" s="20">
+        <f>$G$3+P10+$G$4+P11+$G$5+P12</f>
+        <v>15</v>
+      </c>
+      <c r="Q13" s="20">
+        <f>Q12+$H$5+Q11+$H$4+Q10+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="R13" s="20">
+        <f>R12+$I$5+R11+$I$4+R10+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="S13" s="20">
+        <f>$G$3+P10+$H$4+Q11+$I$5+R12</f>
+        <v>15</v>
+      </c>
+      <c r="U13" t="s">
         <v>28</v>
       </c>
-      <c r="V12">
-        <f>((V10)+1)^2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="14">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="L13" t="s">
+      <c r="V13">
+        <f>((V11)+1)^2</f>
+        <v>1</v>
+      </c>
+      <c r="X13" s="20">
+        <f>Y12+Z11+AA10+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="Y13" s="20">
+        <f>$G$3+Y10+$G$4+Y11+$G$5+Y12</f>
+        <v>15</v>
+      </c>
+      <c r="Z13" s="20">
+        <f>Z12+$H$5+Z11+$H$4+Z10+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="AA13" s="20">
+        <f>AA12+$I$5+AA11+$I$4+AA10+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="AB13" s="20">
+        <f>$G$3+Y10+$H$4+Z11+$I$5+AA12</f>
+        <v>15</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE13">
+        <f>((AE11)+1)^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="L14" t="s">
         <v>30</v>
       </c>
-      <c r="M13">
-        <f>(M10+M11)*M12</f>
+      <c r="M14">
+        <f>(M11+M12)*M13</f>
         <v>7</v>
       </c>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="U13" t="s">
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="U14" t="s">
         <v>30</v>
       </c>
-      <c r="V13">
-        <f>(V10+V11)*V12</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15">
-        <v>1</v>
-      </c>
-      <c r="C14" s="16">
-        <v>2</v>
-      </c>
-      <c r="D14" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="13">
-        <v>2</v>
-      </c>
-      <c r="C15" s="14">
-        <v>0</v>
+      <c r="V14">
+        <f>(V11+V12)*V13</f>
+        <v>15</v>
+      </c>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AD14" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE14">
+        <f>(AE11+AE12)*AE13</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="16">
+        <v>2</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="21"/>
     </row>
-    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8">
-        <v>2</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B16" s="13">
+        <v>2</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E16" s="21"/>
-      <c r="L16" s="33" t="s">
+    </row>
+    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8">
+        <v>2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="L17" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M16" s="33"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="18">
-        <v>2</v>
-      </c>
-      <c r="C17" s="19">
-        <v>2</v>
-      </c>
-      <c r="D17" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="22">
-        <v>3</v>
-      </c>
-      <c r="H17" s="23">
-        <v>0</v>
-      </c>
-      <c r="I17" s="24">
-        <v>1</v>
-      </c>
-      <c r="J17" s="20">
-        <f>$G$3+G17+$H$3+H17+$I$3+I17</f>
-        <v>16</v>
-      </c>
-      <c r="L17" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17">
-        <f>IF(J17=15,1,0) + IF(J18=15,1,0) + IF(J19=15,1,0)+ IF(J20=15,1,0)+ IF(I20=15,1,0) + IF(H20=15,1,0) + IF(G20=15,1,0) + IF(F20=15,1,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="33"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="U17" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="V17" s="33"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B18" s="18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="19">
+        <v>2</v>
+      </c>
+      <c r="D18" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E18" s="21"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="25">
-        <v>0</v>
-      </c>
-      <c r="H18" s="26">
-        <v>0</v>
-      </c>
-      <c r="I18" s="27">
+      <c r="G18" s="22">
+        <v>3</v>
+      </c>
+      <c r="H18" s="23">
+        <v>0</v>
+      </c>
+      <c r="I18" s="24">
         <v>1</v>
       </c>
       <c r="J18" s="20">
-        <f>$G$4+G18+$H$4+H18+$I$4+I18</f>
-        <v>15</v>
+        <f>$G$3+G18+$H$3+H18+$I$3+I18</f>
+        <v>16</v>
       </c>
       <c r="L18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18">
+        <f>IF(J18=15,1,0) + IF(J19=15,1,0) + IF(J20=15,1,0)+ IF(J21=15,1,0)+ IF(I21=15,1,0) + IF(H21=15,1,0) + IF(G21=15,1,0) + IF(F21=15,1,0)</f>
+        <v>5</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="P18" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="23">
+        <v>1</v>
+      </c>
+      <c r="R18" s="24">
+        <v>0</v>
+      </c>
+      <c r="S18" s="20">
+        <f>$G$3+P18+$H$3+Q18+$I$3+R18</f>
+        <v>15</v>
+      </c>
+      <c r="U18" t="s">
+        <v>27</v>
+      </c>
+      <c r="V18">
+        <f>IF(S18=15,1,0) + IF(S19=15,1,0) + IF(S20=15,1,0)+ IF(S21=15,1,0)+ IF(R21=15,1,0) + IF(Q21=15,1,0) + IF(P21=15,1,0) + IF(O21=15,1,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="E19" s="21"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="25">
+        <v>0</v>
+      </c>
+      <c r="H19" s="26">
+        <v>0</v>
+      </c>
+      <c r="I19" s="27">
+        <v>1</v>
+      </c>
+      <c r="J19" s="20">
+        <f>$G$4+G19+$H$4+H19+$I$4+I19</f>
+        <v>15</v>
+      </c>
+      <c r="L19" t="s">
         <v>21</v>
       </c>
-      <c r="M18">
-        <f>8-M17</f>
+      <c r="M19">
+        <f>8-M18</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="20"/>
-      <c r="G19" s="28">
-        <v>0</v>
-      </c>
-      <c r="H19" s="29">
+      <c r="O19" s="20"/>
+      <c r="P19" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="26">
+        <v>0</v>
+      </c>
+      <c r="R19" s="27">
+        <v>0</v>
+      </c>
+      <c r="S19" s="20">
+        <f>$G$4+P19+$H$4+Q19+$I$4+R19</f>
+        <v>15</v>
+      </c>
+      <c r="U19" t="s">
+        <v>21</v>
+      </c>
+      <c r="V19">
+        <f>8-V18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="20"/>
+      <c r="G20" s="28">
+        <v>0</v>
+      </c>
+      <c r="H20" s="29">
         <v>3</v>
       </c>
-      <c r="I19" s="30">
-        <v>0</v>
-      </c>
-      <c r="J19" s="20">
-        <f>$G$5+G19+$H$5+H19+$I$5+I19</f>
-        <v>15</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="I20" s="30">
+        <v>0</v>
+      </c>
+      <c r="J20" s="20">
+        <f>$G$5+G20+$H$5+H20+$I$5+I20</f>
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
         <v>22</v>
       </c>
-      <c r="M19">
-        <f>ABS(G17)+ABS(H17)+ABS(I17)+ABS(G18)+ABS(H18)+ABS(I18)+ABS(G19)+ABS(H19)+ABS(I19)</f>
+      <c r="M20">
+        <f>ABS(G18)+ABS(H18)+ABS(I18)+ABS(G19)+ABS(H19)+ABS(I19)+ABS(G20)+ABS(H20)+ABS(I20)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="O20" s="20"/>
+      <c r="P20" s="28">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="29">
+        <v>2</v>
+      </c>
+      <c r="R20" s="30">
+        <v>1</v>
+      </c>
+      <c r="S20" s="20">
+        <f>$G$5+P20+$H$5+Q20+$I$5+R20</f>
+        <v>15</v>
+      </c>
+      <c r="U20" t="s">
+        <v>22</v>
+      </c>
+      <c r="V20">
+        <f>ABS(P18)+ABS(Q18)+ABS(R18)+ABS(P19)+ABS(Q19)+ABS(R19)+ABS(P20)+ABS(Q20)+ABS(R20)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="20">
-        <f>G19+H18+I17+$G$5+$H$4+$I$3</f>
+      <c r="F21" s="20">
+        <f>G20+H19+I18+$G$5+$H$4+$I$3</f>
         <v>16</v>
       </c>
-      <c r="G20" s="20">
-        <f>$G$3+G17+$G$4+G18+$G$5+G19</f>
-        <v>15</v>
-      </c>
-      <c r="H20" s="20">
-        <f>H19+$H$5+H18+$H$4+H17+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="I20" s="20">
-        <f>I19+$I$5+I18+$I$4+I17+$I$3</f>
+      <c r="G21" s="20">
+        <f>$G$3+G18+$G$4+G19+$G$5+G20</f>
+        <v>15</v>
+      </c>
+      <c r="H21" s="20">
+        <f>H20+$H$5+H19+$H$4+H18+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="I21" s="20">
+        <f>I20+$I$5+I19+$I$4+I18+$I$3</f>
         <v>16</v>
       </c>
-      <c r="J20" s="20">
-        <f>$G$3+G17+$H$4+H18+$I$5+I19</f>
-        <v>15</v>
-      </c>
-      <c r="L20" t="s">
+      <c r="J21" s="20">
+        <f>$G$3+G18+$H$4+H19+$I$5+I20</f>
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
         <v>28</v>
       </c>
-      <c r="M20">
-        <f>((M18)+1)^2</f>
+      <c r="M21">
+        <f>((M19)+1)^2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L21" t="s">
+      <c r="O21" s="20">
+        <f>P20+Q19+R18+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="P21" s="20">
+        <f>$G$3+P18+$G$4+P19+$G$5+P20</f>
+        <v>15</v>
+      </c>
+      <c r="Q21" s="20">
+        <f>Q20+$H$5+Q19+$H$4+Q18+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="R21" s="20">
+        <f>R20+$I$5+R19+$I$4+R18+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="S21" s="20">
+        <f>$G$3+P18+$H$4+Q19+$I$5+R20</f>
+        <v>15</v>
+      </c>
+      <c r="U21" t="s">
+        <v>28</v>
+      </c>
+      <c r="V21">
+        <f>((V19)+1)^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
         <v>30</v>
       </c>
-      <c r="M21">
-        <f>(M18+M19)*M20</f>
+      <c r="M22">
+        <f>(M19+M20)*M21</f>
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L24" s="33" t="s">
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="U22" t="s">
+        <v>30</v>
+      </c>
+      <c r="V22">
+        <f>(V19+V20)*V21</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M24" s="33"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F25" s="20"/>
-      <c r="G25" s="22">
+      <c r="M25" s="33"/>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F26" s="20"/>
+      <c r="G26" s="22">
         <v>3</v>
       </c>
-      <c r="H25" s="23">
-        <v>0</v>
-      </c>
-      <c r="I25" s="24">
+      <c r="H26" s="23">
+        <v>0</v>
+      </c>
+      <c r="I26" s="24">
         <v>-1</v>
       </c>
-      <c r="J25" s="20">
-        <f>$G$3+G25+$H$3+H25+$I$3+I25</f>
+      <c r="J26" s="20">
+        <f>$G$3+G26+$H$3+H26+$I$3+I26</f>
         <v>14</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L26" t="s">
         <v>27</v>
       </c>
-      <c r="M25">
-        <f>IF(J25=15,1,0) + IF(J26=15,1,0) + IF(J27=15,1,0)+ IF(J28=15,1,0)+ IF(I28=15,1,0) + IF(H28=15,1,0) + IF(G28=15,1,0) + IF(F28=15,1,0)</f>
+      <c r="M26">
+        <f>IF(J26=15,1,0) + IF(J27=15,1,0) + IF(J28=15,1,0)+ IF(J29=15,1,0)+ IF(I29=15,1,0) + IF(H29=15,1,0) + IF(G29=15,1,0) + IF(F29=15,1,0)</f>
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F26" s="20"/>
-      <c r="G26" s="25">
-        <v>0</v>
-      </c>
-      <c r="H26" s="26">
-        <v>0</v>
-      </c>
-      <c r="I26" s="27">
-        <v>1</v>
-      </c>
-      <c r="J26" s="20">
-        <f>$G$4+G26+$H$4+H26+$I$4+I26</f>
-        <v>15</v>
-      </c>
-      <c r="L26" t="s">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F27" s="20"/>
+      <c r="G27" s="25">
+        <v>0</v>
+      </c>
+      <c r="H27" s="26">
+        <v>0</v>
+      </c>
+      <c r="I27" s="27">
+        <v>1</v>
+      </c>
+      <c r="J27" s="20">
+        <f>$G$4+G27+$H$4+H27+$I$4+I27</f>
+        <v>15</v>
+      </c>
+      <c r="L27" t="s">
         <v>21</v>
       </c>
-      <c r="M26">
-        <f>8-M25</f>
+      <c r="M27">
+        <f>8-M26</f>
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="20"/>
-      <c r="G27" s="28">
-        <v>0</v>
-      </c>
-      <c r="H27" s="29">
+    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="20"/>
+      <c r="G28" s="28">
+        <v>0</v>
+      </c>
+      <c r="H28" s="29">
         <v>3</v>
       </c>
-      <c r="I27" s="30">
-        <v>0</v>
-      </c>
-      <c r="J27" s="20">
-        <f>$G$5+G27+$H$5+H27+$I$5+I27</f>
-        <v>15</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="I28" s="30">
+        <v>0</v>
+      </c>
+      <c r="J28" s="20">
+        <f>$G$5+G28+$H$5+H28+$I$5+I28</f>
+        <v>15</v>
+      </c>
+      <c r="L28" t="s">
         <v>22</v>
       </c>
-      <c r="M27">
-        <f>ABS(G25)+ABS(H25)+ABS(I25)+ABS(G26)+ABS(H26)+ABS(I26)+ABS(G27)+ABS(H27)+ABS(I27)</f>
+      <c r="M28">
+        <f>ABS(G26)+ABS(H26)+ABS(I26)+ABS(G27)+ABS(H27)+ABS(I27)+ABS(G28)+ABS(H28)+ABS(I28)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F28" s="20">
-        <f>G27+H26+I25+$G$5+$H$4+$I$3</f>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="F29" s="20">
+        <f>G28+H27+I26+$G$5+$H$4+$I$3</f>
         <v>14</v>
       </c>
-      <c r="G28" s="20">
-        <f>$G$3+G25+$G$4+G26+$G$5+G27</f>
-        <v>15</v>
-      </c>
-      <c r="H28" s="20">
-        <f>H27+$H$5+H26+$H$4+H25+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="I28" s="20">
-        <f>I27+$I$5+I26+$I$4+I25+$I$3</f>
+      <c r="G29" s="20">
+        <f>$G$3+G26+$G$4+G27+$G$5+G28</f>
+        <v>15</v>
+      </c>
+      <c r="H29" s="20">
+        <f>H28+$H$5+H27+$H$4+H26+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="I29" s="20">
+        <f>I28+$I$5+I27+$I$4+I26+$I$3</f>
         <v>14</v>
       </c>
-      <c r="J28" s="20">
-        <f>$G$3+G25+$H$4+H26+$I$5+I27</f>
-        <v>15</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="J29" s="20">
+        <f>$G$3+G26+$H$4+H27+$I$5+I28</f>
+        <v>15</v>
+      </c>
+      <c r="L29" t="s">
         <v>28</v>
       </c>
-      <c r="M28">
-        <f>((M26)+1)^2</f>
+      <c r="M29">
+        <f>((M27)+1)^2</f>
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="L29" t="s">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
         <v>30</v>
       </c>
-      <c r="M29">
-        <f>(M26+M27)*M28</f>
+      <c r="M30">
+        <f>(M27+M28)*M29</f>
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="33" t="s">
+    <row r="33" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L33" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M32" s="33"/>
-    </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F33" s="20"/>
-      <c r="G33" s="22">
-        <v>1</v>
-      </c>
-      <c r="H33" s="23">
-        <v>0</v>
-      </c>
-      <c r="I33" s="24">
-        <v>-1</v>
-      </c>
-      <c r="J33" s="20">
-        <f>$G$3+G33+$H$3+H33+$I$3+I33</f>
-        <v>12</v>
-      </c>
-      <c r="L33" t="s">
-        <v>27</v>
-      </c>
-      <c r="M33">
-        <f>IF(J33=15,1,0) + IF(J34=15,1,0) + IF(J35=15,1,0)+ IF(J36=15,1,0)+ IF(I36=15,1,0) + IF(H36=15,1,0) + IF(G36=15,1,0) + IF(F36=15,1,0)</f>
-        <v>2</v>
-      </c>
+      <c r="M33" s="33"/>
     </row>
     <row r="34" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F34" s="20"/>
-      <c r="G34" s="25">
-        <v>1</v>
-      </c>
-      <c r="H34" s="26">
-        <v>0</v>
-      </c>
-      <c r="I34" s="27">
-        <v>1</v>
+      <c r="G34" s="22">
+        <v>1</v>
+      </c>
+      <c r="H34" s="23">
+        <v>0</v>
+      </c>
+      <c r="I34" s="24">
+        <v>-1</v>
       </c>
       <c r="J34" s="20">
-        <f>$G$4+G34+$H$4+H34+$I$4+I34</f>
+        <f>$G$3+G34+$H$3+H34+$I$3+I34</f>
+        <v>12</v>
+      </c>
+      <c r="L34" t="s">
+        <v>27</v>
+      </c>
+      <c r="M34">
+        <f>IF(J34=15,1,0) + IF(J35=15,1,0) + IF(J36=15,1,0)+ IF(J37=15,1,0)+ IF(I37=15,1,0) + IF(H37=15,1,0) + IF(G37=15,1,0) + IF(F37=15,1,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F35" s="20"/>
+      <c r="G35" s="25">
+        <v>1</v>
+      </c>
+      <c r="H35" s="26">
+        <v>0</v>
+      </c>
+      <c r="I35" s="27">
+        <v>1</v>
+      </c>
+      <c r="J35" s="20">
+        <f>$G$4+G35+$H$4+H35+$I$4+I35</f>
         <v>16</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L35" t="s">
         <v>21</v>
       </c>
-      <c r="M34">
-        <f>8-M33</f>
+      <c r="M35">
+        <f>8-M34</f>
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="20"/>
-      <c r="G35" s="28">
-        <v>0</v>
-      </c>
-      <c r="H35" s="29">
-        <v>1</v>
-      </c>
-      <c r="I35" s="30">
-        <v>2</v>
-      </c>
-      <c r="J35" s="20">
-        <f>$G$5+G35+$H$5+H35+$I$5+I35</f>
-        <v>15</v>
-      </c>
-      <c r="L35" t="s">
+    <row r="36" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="20"/>
+      <c r="G36" s="28">
+        <v>0</v>
+      </c>
+      <c r="H36" s="29">
+        <v>1</v>
+      </c>
+      <c r="I36" s="30">
+        <v>2</v>
+      </c>
+      <c r="J36" s="20">
+        <f>$G$5+G36+$H$5+H36+$I$5+I36</f>
+        <v>15</v>
+      </c>
+      <c r="L36" t="s">
         <v>22</v>
       </c>
-      <c r="M35">
-        <f>ABS(G33)+ABS(H33)+ABS(I33)+ABS(G34)+ABS(H34)+ABS(I34)+ABS(G35)+ABS(H35)+ABS(I35)</f>
+      <c r="M36">
+        <f>ABS(G34)+ABS(H34)+ABS(I34)+ABS(G35)+ABS(H35)+ABS(I35)+ABS(G36)+ABS(H36)+ABS(I36)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F36" s="20">
-        <f>G35+H34+I33+$G$5+$H$4+$I$3</f>
+    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F37" s="20">
+        <f>G36+H35+I34+$G$5+$H$4+$I$3</f>
         <v>14</v>
       </c>
-      <c r="G36" s="20">
-        <f>$G$3+G33+$G$4+G34+$G$5+G35</f>
+      <c r="G37" s="20">
+        <f>$G$3+G34+$G$4+G35+$G$5+G36</f>
         <v>14</v>
       </c>
-      <c r="H36" s="20">
-        <f>H35+$H$5+H34+$H$4+H33+$H$3</f>
+      <c r="H37" s="20">
+        <f>H36+$H$5+H35+$H$4+H34+$H$3</f>
         <v>13</v>
       </c>
-      <c r="I36" s="20">
-        <f>I35+$I$5+I34+$I$4+I33+$I$3</f>
+      <c r="I37" s="20">
+        <f>I36+$I$5+I35+$I$4+I34+$I$3</f>
         <v>16</v>
       </c>
-      <c r="J36" s="20">
-        <f>$G$3+G33+$H$4+H34+$I$5+I35</f>
-        <v>15</v>
-      </c>
-      <c r="L36" t="s">
+      <c r="J37" s="20">
+        <f>$G$3+G34+$H$4+H35+$I$5+I36</f>
+        <v>15</v>
+      </c>
+      <c r="L37" t="s">
         <v>28</v>
       </c>
-      <c r="M36">
-        <f>((M34)+1)^2</f>
+      <c r="M37">
+        <f>((M35)+1)^2</f>
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L37" t="s">
+    <row r="38" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
         <v>30</v>
       </c>
-      <c r="M37">
-        <f>(M34+M35)*M36</f>
+      <c r="M38">
+        <f>(M35+M36)*M37</f>
         <v>637</v>
       </c>
     </row>
-    <row r="40" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L40" s="33" t="s">
+    <row r="41" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M40" s="33"/>
-    </row>
-    <row r="41" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F41" s="20"/>
-      <c r="G41" s="22">
-        <v>0</v>
-      </c>
-      <c r="H41" s="23">
-        <v>0</v>
-      </c>
-      <c r="I41" s="24">
-        <v>0</v>
-      </c>
-      <c r="J41" s="20">
-        <f>$G$3+G41+$H$3+H41+$I$3+I41</f>
-        <v>12</v>
-      </c>
-      <c r="L41" t="s">
-        <v>27</v>
-      </c>
-      <c r="M41">
-        <f>IF(J41=15,1,0) + IF(J42=15,1,0) + IF(J43=15,1,0)+ IF(J44=15,1,0)+ IF(I44=15,1,0) + IF(H44=15,1,0) + IF(G44=15,1,0) + IF(F44=15,1,0)</f>
-        <v>2</v>
-      </c>
+      <c r="M41" s="33"/>
     </row>
     <row r="42" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F42" s="20"/>
-      <c r="G42" s="25">
-        <v>1</v>
-      </c>
-      <c r="H42" s="26">
-        <v>0</v>
-      </c>
-      <c r="I42" s="27">
+      <c r="G42" s="22">
+        <v>0</v>
+      </c>
+      <c r="H42" s="23">
+        <v>0</v>
+      </c>
+      <c r="I42" s="24">
         <v>0</v>
       </c>
       <c r="J42" s="20">
-        <f>$G$4+G42+$H$4+H42+$I$4+I42</f>
-        <v>15</v>
+        <f>$G$3+G42+$H$3+H42+$I$3+I42</f>
+        <v>12</v>
       </c>
       <c r="L42" t="s">
+        <v>27</v>
+      </c>
+      <c r="M42">
+        <f>IF(J42=15,1,0) + IF(J43=15,1,0) + IF(J44=15,1,0)+ IF(J45=15,1,0)+ IF(I45=15,1,0) + IF(H45=15,1,0) + IF(G45=15,1,0) + IF(F45=15,1,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F43" s="20"/>
+      <c r="G43" s="25">
+        <v>1</v>
+      </c>
+      <c r="H43" s="26">
+        <v>0</v>
+      </c>
+      <c r="I43" s="27">
+        <v>0</v>
+      </c>
+      <c r="J43" s="20">
+        <f>$G$4+G43+$H$4+H43+$I$4+I43</f>
+        <v>15</v>
+      </c>
+      <c r="L43" t="s">
         <v>21</v>
       </c>
-      <c r="M42">
-        <f>8-M41</f>
+      <c r="M43">
+        <f>8-M42</f>
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="20"/>
-      <c r="G43" s="28">
-        <v>0</v>
-      </c>
-      <c r="H43" s="29">
-        <v>0</v>
-      </c>
-      <c r="I43" s="30">
-        <v>0</v>
-      </c>
-      <c r="J43" s="20">
-        <f>$G$5+G43+$H$5+H43+$I$5+I43</f>
+    <row r="44" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F44" s="20"/>
+      <c r="G44" s="28">
+        <v>0</v>
+      </c>
+      <c r="H44" s="29">
+        <v>0</v>
+      </c>
+      <c r="I44" s="30">
+        <v>0</v>
+      </c>
+      <c r="J44" s="20">
+        <f>$G$5+G44+$H$5+H44+$I$5+I44</f>
         <v>12</v>
       </c>
-      <c r="L43" t="s">
+      <c r="L44" t="s">
         <v>22</v>
       </c>
-      <c r="M43">
-        <f>ABS(G41)+ABS(H41)+ABS(I41)+ABS(G42)+ABS(H42)+ABS(I42)+ABS(G43)+ABS(H43)+ABS(I43)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F44" s="20">
-        <f>G43+H42+I41+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="G44" s="20">
-        <f>$G$3+G41+$G$4+G42+$G$5+G43</f>
+      <c r="M44">
+        <f>ABS(G42)+ABS(H42)+ABS(I42)+ABS(G43)+ABS(H43)+ABS(I43)+ABS(G44)+ABS(H44)+ABS(I44)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F45" s="20">
+        <f>G44+H43+I42+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="G45" s="20">
+        <f>$G$3+G42+$G$4+G43+$G$5+G44</f>
         <v>13</v>
       </c>
-      <c r="H44" s="20">
-        <f>H43+$H$5+H42+$H$4+H41+$H$3</f>
+      <c r="H45" s="20">
+        <f>H44+$H$5+H43+$H$4+H42+$H$3</f>
         <v>12</v>
       </c>
-      <c r="I44" s="20">
-        <f>I43+$I$5+I42+$I$4+I41+$I$3</f>
+      <c r="I45" s="20">
+        <f>I44+$I$5+I43+$I$4+I42+$I$3</f>
         <v>14</v>
       </c>
-      <c r="J44" s="20">
-        <f>$G$3+G41+$H$4+H42+$I$5+I43</f>
+      <c r="J45" s="20">
+        <f>$G$3+G42+$H$4+H43+$I$5+I44</f>
         <v>12</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L45" t="s">
         <v>28</v>
       </c>
-      <c r="M44">
-        <f>((M42)+1)^2</f>
+      <c r="M45">
+        <f>((M43)+1)^2</f>
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L45" t="s">
+    <row r="46" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L46" t="s">
         <v>30</v>
       </c>
-      <c r="M45">
-        <f>(M42+M43)*M44</f>
+      <c r="M46">
+        <f>(M43+M44)*M45</f>
         <v>343</v>
       </c>
     </row>
-    <row r="47" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L47" s="33" t="s">
+    <row r="48" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L48" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M47" s="33"/>
-    </row>
-    <row r="48" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F48" s="20"/>
-      <c r="G48" s="22">
-        <v>0</v>
-      </c>
-      <c r="H48" s="23">
-        <v>0</v>
-      </c>
-      <c r="I48" s="24">
-        <v>0</v>
-      </c>
-      <c r="J48" s="20">
-        <f>$G$3+G48+$H$3+H48+$I$3+I48</f>
-        <v>12</v>
-      </c>
-      <c r="L48" t="s">
-        <v>27</v>
-      </c>
-      <c r="M48">
-        <f>IF(J48=15,1,0) + IF(J49=15,1,0) + IF(J50=15,1,0)+ IF(J51=15,1,0)+ IF(I51=15,1,0) + IF(H51=15,1,0) + IF(G51=15,1,0) + IF(F51=15,1,0)</f>
-        <v>1</v>
-      </c>
+      <c r="M48" s="33"/>
     </row>
     <row r="49" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F49" s="20"/>
-      <c r="G49" s="25">
-        <v>0</v>
-      </c>
-      <c r="H49" s="26">
-        <v>0</v>
-      </c>
-      <c r="I49" s="27">
+      <c r="G49" s="22">
+        <v>0</v>
+      </c>
+      <c r="H49" s="23">
+        <v>0</v>
+      </c>
+      <c r="I49" s="24">
         <v>0</v>
       </c>
       <c r="J49" s="20">
-        <f>$G$4+G49+$H$4+H49+$I$4+I49</f>
+        <f>$G$3+G49+$H$3+H49+$I$3+I49</f>
+        <v>12</v>
+      </c>
+      <c r="L49" t="s">
+        <v>27</v>
+      </c>
+      <c r="M49">
+        <f>IF(J49=15,1,0) + IF(J50=15,1,0) + IF(J51=15,1,0)+ IF(J52=15,1,0)+ IF(I52=15,1,0) + IF(H52=15,1,0) + IF(G52=15,1,0) + IF(F52=15,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F50" s="20"/>
+      <c r="G50" s="25">
+        <v>0</v>
+      </c>
+      <c r="H50" s="26">
+        <v>0</v>
+      </c>
+      <c r="I50" s="27">
+        <v>0</v>
+      </c>
+      <c r="J50" s="20">
+        <f>$G$4+G50+$H$4+H50+$I$4+I50</f>
         <v>14</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L50" t="s">
         <v>21</v>
       </c>
-      <c r="M49">
-        <f>8-M48</f>
+      <c r="M50">
+        <f>8-M49</f>
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F50" s="20"/>
-      <c r="G50" s="28">
-        <v>0</v>
-      </c>
-      <c r="H50" s="29">
-        <v>0</v>
-      </c>
-      <c r="I50" s="30">
-        <v>0</v>
-      </c>
-      <c r="J50" s="20">
-        <f>$G$5+G50+$H$5+H50+$I$5+I50</f>
+    <row r="51" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F51" s="20"/>
+      <c r="G51" s="28">
+        <v>0</v>
+      </c>
+      <c r="H51" s="29">
+        <v>0</v>
+      </c>
+      <c r="I51" s="30">
+        <v>0</v>
+      </c>
+      <c r="J51" s="20">
+        <f>$G$5+G51+$H$5+H51+$I$5+I51</f>
         <v>12</v>
       </c>
-      <c r="L50" t="s">
+      <c r="L51" t="s">
         <v>22</v>
       </c>
-      <c r="M50">
-        <f>ABS(G48)+ABS(H48)+ABS(I48)+ABS(G49)+ABS(H49)+ABS(I49)+ABS(G50)+ABS(H50)+ABS(I50)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F51" s="20">
-        <f>G50+H49+I48+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="G51" s="20">
-        <f>$G$3+G48+$G$4+G49+$G$5+G50</f>
+      <c r="M51">
+        <f>ABS(G49)+ABS(H49)+ABS(I49)+ABS(G50)+ABS(H50)+ABS(I50)+ABS(G51)+ABS(H51)+ABS(I51)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F52" s="20">
+        <f>G51+H50+I49+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="G52" s="20">
+        <f>$G$3+G49+$G$4+G50+$G$5+G51</f>
         <v>12</v>
       </c>
-      <c r="H51" s="20">
-        <f>H50+$H$5+H49+$H$4+H48+$H$3</f>
+      <c r="H52" s="20">
+        <f>H51+$H$5+H50+$H$4+H49+$H$3</f>
         <v>12</v>
       </c>
-      <c r="I51" s="20">
-        <f>I50+$I$5+I49+$I$4+I48+$I$3</f>
+      <c r="I52" s="20">
+        <f>I51+$I$5+I50+$I$4+I49+$I$3</f>
         <v>14</v>
       </c>
-      <c r="J51" s="20">
-        <f>$G$3+G48+$H$4+H49+$I$5+I50</f>
+      <c r="J52" s="20">
+        <f>$G$3+G49+$H$4+H50+$I$5+I51</f>
         <v>12</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L52" t="s">
         <v>28</v>
       </c>
-      <c r="M51">
-        <f>((M49)+1)^2</f>
+      <c r="M52">
+        <f>((M50)+1)^2</f>
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L52" t="s">
+    <row r="53" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L53" t="s">
         <v>30</v>
       </c>
-      <c r="M52">
-        <f>(M49+M50)*M51</f>
+      <c r="M53">
+        <f>(M50+M51)*M52</f>
         <v>448</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="U8:V8"/>
+  <mergeCells count="10">
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="AD9:AE9"/>
+    <mergeCell ref="U17:V17"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="L41:M41"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J3:J6 F6:I6">
+  <conditionalFormatting sqref="J3:J7 F6:I7">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J13 F13:I13">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:J21 F21:I21">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26:J29 F29:I29">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34:J37 F37:I37">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9:J12 F12:I12">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+  <conditionalFormatting sqref="J42:J45 F45:I45">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J17:J20 F20:I20">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+  <conditionalFormatting sqref="J49:J52 F52:I52">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:J28 F28:I28">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="S10:S13 O13:R13">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J33:J36 F36:I36">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+  <conditionalFormatting sqref="AB10:AB13 X13:AA13">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J41:J44 F44:I44">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
-      <formula>15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J48:J51 F51:I51">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S9:S12 O12:R12">
+  <conditionalFormatting sqref="S18:S21 O21:R21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>15</formula>
     </cfRule>

</xml_diff>

<commit_message>
Revert "Added crossover, mutation, logging & exit conditions"
This reverts commit 84ede07bc66d31dca6328e189a821df9487afc8e.
</commit_message>
<xml_diff>
--- a/Magic Square/Workbook.xlsx
+++ b/Magic Square/Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callu\Documents\Study\HackerRank\Magic Square\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A455161F-6755-4FF2-8129-C71E8E3BAEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9AA174-40FF-4233-8A52-039F24E670AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2505" windowWidth="21600" windowHeight="11100" xr2:uid="{BF84A0E7-C787-466B-84A6-9C6B3CD38009}"/>
+    <workbookView xWindow="-26085" yWindow="3090" windowWidth="21600" windowHeight="11100" xr2:uid="{BF84A0E7-C787-466B-84A6-9C6B3CD38009}"/>
   </bookViews>
   <sheets>
     <sheet name="3x3" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="33">
   <si>
     <t>column</t>
   </si>
@@ -452,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -552,55 +552,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1021,10 +978,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4129BD6B-3B7F-431A-A917-19F89FB650CA}">
-  <dimension ref="B2:AE53"/>
+  <dimension ref="B2:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,17 +993,15 @@
     <col min="12" max="12" width="9.140625" customWidth="1"/>
     <col min="15" max="19" width="3" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3" customWidth="1"/>
-    <col min="24" max="28" width="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L2" s="33" t="s">
         <v>31</v>
       </c>
       <c r="M2" s="33"/>
     </row>
-    <row r="3" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1075,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>0</v>
       </c>
@@ -1104,7 +1059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <v>1</v>
       </c>
@@ -1126,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6" s="18">
         <v>2</v>
       </c>
@@ -1154,1203 +1109,960 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="9" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="7" t="s">
+    <row r="8" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="L9" s="33" t="s">
+      <c r="E8" s="1"/>
+      <c r="L8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="33"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="U9" s="33" t="s">
+      <c r="M8" s="33"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="U8" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="V9" s="33"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AD9" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE9" s="33"/>
-    </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="V8" s="33"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9">
+        <f>ABS(B9-(3-1))</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="22">
+        <v>3</v>
+      </c>
+      <c r="H9" s="23">
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <v>0</v>
+      </c>
+      <c r="J9" s="20">
+        <f>$G$3+G9+$H$3+H9+$I$3+I9</f>
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M9">
+        <f>IF(J9=15,1,0) + IF(J10=15,1,0) + IF(J11=15,1,0)+ IF(J12=15,1,0)+ IF(I12=15,1,0) + IF(H12=15,1,0) + IF(G12=15,1,0) + IF(F12=15,1,0)</f>
+        <v>8</v>
+      </c>
+      <c r="O9" s="20"/>
+      <c r="P9" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>2</v>
+      </c>
+      <c r="R9" s="24">
+        <v>1</v>
+      </c>
+      <c r="S9" s="20">
+        <f>$G$3+P9+$H$3+Q9+$I$3+R9</f>
+        <v>15</v>
+      </c>
+      <c r="U9" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9">
+        <f>IF(S9=15,1,0) + IF(S10=15,1,0) + IF(S11=15,1,0)+ IF(S12=15,1,0)+ IF(R12=15,1,0) + IF(Q12=15,1,0) + IF(P12=15,1,0) + IF(O12=15,1,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>0</v>
       </c>
       <c r="C10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="9">
-        <f>ABS(B10-(3-1))</f>
+        <f t="shared" ref="D10:D17" si="0">ABS(B10-(3-1))</f>
         <v>2</v>
       </c>
       <c r="E10" s="21"/>
       <c r="F10" s="20"/>
-      <c r="G10" s="22">
-        <v>3</v>
-      </c>
-      <c r="H10" s="23">
-        <v>0</v>
-      </c>
-      <c r="I10" s="24">
-        <v>0</v>
+      <c r="G10" s="25">
+        <v>0</v>
+      </c>
+      <c r="H10" s="26">
+        <v>0</v>
+      </c>
+      <c r="I10" s="27">
+        <v>1</v>
       </c>
       <c r="J10" s="20">
-        <f>$G$3+G10+$H$3+H10+$I$3+I10</f>
+        <f>$G$4+G10+$H$4+H10+$I$4+I10</f>
         <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="M10">
-        <f>IF(J10=15,1,0) + IF(J11=15,1,0) + IF(J12=15,1,0)+ IF(J13=15,1,0)+ IF(I13=15,1,0) + IF(H13=15,1,0) + IF(G13=15,1,0) + IF(F13=15,1,0)</f>
-        <v>8</v>
+        <f>8-M9</f>
+        <v>0</v>
       </c>
       <c r="O10" s="20"/>
-      <c r="P10" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="23">
-        <v>2</v>
-      </c>
-      <c r="R10" s="24">
-        <v>1</v>
+      <c r="P10" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>0</v>
+      </c>
+      <c r="R10" s="27">
+        <v>-3</v>
       </c>
       <c r="S10" s="20">
-        <f>$G$3+P10+$H$3+Q10+$I$3+R10</f>
+        <f>$G$4+P10+$H$4+Q10+$I$4+R10</f>
         <v>15</v>
       </c>
       <c r="U10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="V10">
-        <f>IF(S10=15,1,0) + IF(S11=15,1,0) + IF(S12=15,1,0)+ IF(S13=15,1,0)+ IF(R13=15,1,0) + IF(Q13=15,1,0) + IF(P13=15,1,0) + IF(O13=15,1,0)</f>
-        <v>8</v>
-      </c>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="23">
-        <v>2</v>
-      </c>
-      <c r="AA10" s="24">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="20">
-        <f>$G$3+Y10+$H$3+Z10+$I$3+AA10</f>
-        <v>15</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE10">
-        <f>IF(AB10=15,1,0) + IF(AB11=15,1,0) + IF(AB12=15,1,0)+ IF(AB13=15,1,0)+ IF(AA13=15,1,0) + IF(Z13=15,1,0) + IF(Y13=15,1,0) + IF(X13=15,1,0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
-        <v>0</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
+        <f>8-V9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="11">
+        <v>2</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" ref="D11:D18" si="0">ABS(B11-(3-1))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="20"/>
-      <c r="G11" s="25">
-        <v>0</v>
-      </c>
-      <c r="H11" s="26">
-        <v>0</v>
-      </c>
-      <c r="I11" s="27">
-        <v>1</v>
+      <c r="G11" s="28">
+        <v>0</v>
+      </c>
+      <c r="H11" s="29">
+        <v>3</v>
+      </c>
+      <c r="I11" s="30">
+        <v>0</v>
       </c>
       <c r="J11" s="20">
-        <f>$G$4+G11+$H$4+H11+$I$4+I11</f>
+        <f>$G$5+G11+$H$5+H11+$I$5+I11</f>
         <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M11">
-        <f>8-M10</f>
-        <v>0</v>
+        <f>ABS(G9)+ABS(H9)+ABS(I9)+ABS(G10)+ABS(H10)+ABS(I10)+ABS(G11)+ABS(H11)+ABS(I11)</f>
+        <v>7</v>
       </c>
       <c r="O11" s="20"/>
-      <c r="P11" s="25">
-        <v>4</v>
-      </c>
-      <c r="Q11" s="26">
-        <v>0</v>
-      </c>
-      <c r="R11" s="27">
-        <v>-3</v>
+      <c r="P11" s="28">
+        <v>-1</v>
+      </c>
+      <c r="Q11" s="29">
+        <v>1</v>
+      </c>
+      <c r="R11" s="30">
+        <v>3</v>
       </c>
       <c r="S11" s="20">
-        <f>$G$4+P11+$H$4+Q11+$I$4+R11</f>
+        <f>$G$5+P11+$H$5+Q11+$I$5+R11</f>
         <v>15</v>
       </c>
       <c r="U11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V11">
-        <f>8-V10</f>
-        <v>0</v>
-      </c>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="25">
-        <v>4</v>
-      </c>
-      <c r="Z11" s="26">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="27">
-        <v>-3</v>
-      </c>
-      <c r="AB11" s="20">
-        <f>$G$4+Y11+$H$4+Z11+$I$4+AA11</f>
-        <v>15</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE11">
-        <f>8-AE10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10">
-        <v>0</v>
-      </c>
-      <c r="C12" s="11">
-        <v>2</v>
+        <f>ABS(P9)+ABS(Q9)+ABS(R9)+ABS(P10)+ABS(Q10)+ABS(R10)+ABS(P11)+ABS(Q11)+ABS(R11)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="21"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="28">
-        <v>0</v>
-      </c>
-      <c r="H12" s="29">
+      <c r="F12" s="20">
+        <f>G11+H10+I9+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="G12" s="20">
+        <f>$G$3+G9+$G$4+G10+$G$5+G11</f>
+        <v>15</v>
+      </c>
+      <c r="H12" s="20">
+        <f>H11+$H$5+H10+$H$4+H9+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="I12" s="20">
+        <f>I11+$I$5+I10+$I$4+I9+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="J12" s="20">
+        <f>$G$3+G9+$H$4+H10+$I$5+I11</f>
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12">
+        <f>((M10)+1)^2</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="20">
+        <f>P11+Q10+R9+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="P12" s="20">
+        <f>$G$3+P9+$G$4+P10+$G$5+P11</f>
+        <v>15</v>
+      </c>
+      <c r="Q12" s="20">
+        <f>Q11+$H$5+Q10+$H$4+Q9+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="R12" s="20">
+        <f>R11+$I$5+R10+$I$4+R9+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="S12" s="20">
+        <f>$G$3+P9+$H$4+Q10+$I$5+R11</f>
+        <v>15</v>
+      </c>
+      <c r="U12" t="s">
+        <v>28</v>
+      </c>
+      <c r="V12">
+        <f>((V10)+1)^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="L13" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13">
+        <f>(M10+M11)*M12</f>
+        <v>7</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="U13" t="s">
+        <v>30</v>
+      </c>
+      <c r="V13">
+        <f>(V10+V11)*V12</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15">
+        <v>1</v>
+      </c>
+      <c r="C14" s="16">
+        <v>2</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="L16" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" s="33"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="18">
+        <v>2</v>
+      </c>
+      <c r="C17" s="19">
+        <v>2</v>
+      </c>
+      <c r="D17" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22">
         <v>3</v>
       </c>
-      <c r="I12" s="30">
-        <v>0</v>
-      </c>
-      <c r="J12" s="20">
-        <f>$G$5+G12+$H$5+H12+$I$5+I12</f>
-        <v>15</v>
-      </c>
-      <c r="L12" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12">
-        <f>ABS(G10)+ABS(H10)+ABS(I10)+ABS(G11)+ABS(H11)+ABS(I11)+ABS(G12)+ABS(H12)+ABS(I12)</f>
-        <v>7</v>
-      </c>
-      <c r="O12" s="20"/>
-      <c r="P12" s="28">
-        <v>-1</v>
-      </c>
-      <c r="Q12" s="29">
-        <v>1</v>
-      </c>
-      <c r="R12" s="30">
-        <v>3</v>
-      </c>
-      <c r="S12" s="20">
-        <f>$G$5+P12+$H$5+Q12+$I$5+R12</f>
-        <v>15</v>
-      </c>
-      <c r="U12" t="s">
-        <v>22</v>
-      </c>
-      <c r="V12">
-        <f>ABS(P10)+ABS(Q10)+ABS(R10)+ABS(P11)+ABS(Q11)+ABS(R11)+ABS(P12)+ABS(Q12)+ABS(R12)</f>
-        <v>15</v>
-      </c>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="28">
-        <v>-1</v>
-      </c>
-      <c r="Z12" s="29">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="30">
-        <v>3</v>
-      </c>
-      <c r="AB12" s="20">
-        <f>$G$5+Y12+$H$5+Z12+$I$5+AA12</f>
-        <v>15</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE12">
-        <f>ABS(Y10)+ABS(Z10)+ABS(AA10)+ABS(Y11)+ABS(Z11)+ABS(AA11)+ABS(Y12)+ABS(Z12)+ABS(AA12)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>0</v>
-      </c>
-      <c r="D13" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="20">
-        <f>G12+H11+I10+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="G13" s="20">
-        <f>$G$3+G10+$G$4+G11+$G$5+G12</f>
-        <v>15</v>
-      </c>
-      <c r="H13" s="20">
-        <f>H12+$H$5+H11+$H$4+H10+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="I13" s="20">
-        <f>I12+$I$5+I11+$I$4+I10+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="J13" s="20">
-        <f>$G$3+G10+$H$4+H11+$I$5+I12</f>
-        <v>15</v>
-      </c>
-      <c r="L13" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13">
-        <f>((M11)+1)^2</f>
-        <v>1</v>
-      </c>
-      <c r="O13" s="20">
-        <f>P12+Q11+R10+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="P13" s="20">
-        <f>$G$3+P10+$G$4+P11+$G$5+P12</f>
-        <v>15</v>
-      </c>
-      <c r="Q13" s="20">
-        <f>Q12+$H$5+Q11+$H$4+Q10+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="R13" s="20">
-        <f>R12+$I$5+R11+$I$4+R10+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="S13" s="20">
-        <f>$G$3+P10+$H$4+Q11+$I$5+R12</f>
-        <v>15</v>
-      </c>
-      <c r="U13" t="s">
-        <v>28</v>
-      </c>
-      <c r="V13">
-        <f>((V11)+1)^2</f>
-        <v>1</v>
-      </c>
-      <c r="X13" s="20">
-        <f>Y12+Z11+AA10+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="Y13" s="20">
-        <f>$G$3+Y10+$G$4+Y11+$G$5+Y12</f>
-        <v>15</v>
-      </c>
-      <c r="Z13" s="20">
-        <f>Z12+$H$5+Z11+$H$4+Z10+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="AA13" s="20">
-        <f>AA12+$I$5+AA11+$I$4+AA10+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="AB13" s="20">
-        <f>$G$3+Y10+$H$4+Z11+$I$5+AA12</f>
-        <v>15</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE13">
-        <f>((AE11)+1)^2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="L14" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14">
-        <f>(M11+M12)*M13</f>
-        <v>7</v>
-      </c>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="U14" t="s">
-        <v>30</v>
-      </c>
-      <c r="V14">
-        <f>(V11+V12)*V13</f>
-        <v>15</v>
-      </c>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AD14" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE14">
-        <f>(AE11+AE12)*AE13</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="16">
-        <v>2</v>
-      </c>
-      <c r="D15" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="21"/>
-    </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="13">
-        <v>2</v>
-      </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8">
-        <v>2</v>
-      </c>
-      <c r="C17" s="9">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="21"/>
-      <c r="L17" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" s="33"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="U17" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="V17" s="33"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="18">
-        <v>2</v>
-      </c>
-      <c r="C18" s="19">
-        <v>2</v>
-      </c>
-      <c r="D18" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H17" s="23">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24">
+        <v>1</v>
+      </c>
+      <c r="J17" s="20">
+        <f>$G$3+G17+$H$3+H17+$I$3+I17</f>
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17">
+        <f>IF(J17=15,1,0) + IF(J18=15,1,0) + IF(J19=15,1,0)+ IF(J20=15,1,0)+ IF(I20=15,1,0) + IF(H20=15,1,0) + IF(G20=15,1,0) + IF(F20=15,1,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E18" s="21"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="22">
+      <c r="G18" s="25">
+        <v>0</v>
+      </c>
+      <c r="H18" s="26">
+        <v>0</v>
+      </c>
+      <c r="I18" s="27">
+        <v>1</v>
+      </c>
+      <c r="J18" s="20">
+        <f>$G$4+G18+$H$4+H18+$I$4+I18</f>
+        <v>15</v>
+      </c>
+      <c r="L18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18">
+        <f>8-M17</f>
         <v>3</v>
       </c>
-      <c r="H18" s="23">
-        <v>0</v>
-      </c>
-      <c r="I18" s="24">
-        <v>1</v>
-      </c>
-      <c r="J18" s="20">
-        <f>$G$3+G18+$H$3+H18+$I$3+I18</f>
+    </row>
+    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="20"/>
+      <c r="G19" s="28">
+        <v>0</v>
+      </c>
+      <c r="H19" s="29">
+        <v>3</v>
+      </c>
+      <c r="I19" s="30">
+        <v>0</v>
+      </c>
+      <c r="J19" s="20">
+        <f>$G$5+G19+$H$5+H19+$I$5+I19</f>
+        <v>15</v>
+      </c>
+      <c r="L19" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19">
+        <f>ABS(G17)+ABS(H17)+ABS(I17)+ABS(G18)+ABS(H18)+ABS(I18)+ABS(G19)+ABS(H19)+ABS(I19)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="20">
+        <f>G19+H18+I17+$G$5+$H$4+$I$3</f>
         <v>16</v>
       </c>
-      <c r="L18" t="s">
+      <c r="G20" s="20">
+        <f>$G$3+G17+$G$4+G18+$G$5+G19</f>
+        <v>15</v>
+      </c>
+      <c r="H20" s="20">
+        <f>H19+$H$5+H18+$H$4+H17+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="I20" s="20">
+        <f>I19+$I$5+I18+$I$4+I17+$I$3</f>
+        <v>16</v>
+      </c>
+      <c r="J20" s="20">
+        <f>$G$3+G17+$H$4+H18+$I$5+I19</f>
+        <v>15</v>
+      </c>
+      <c r="L20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20">
+        <f>((M18)+1)^2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21">
+        <f>(M18+M19)*M20</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M24" s="33"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F25" s="20"/>
+      <c r="G25" s="22">
+        <v>3</v>
+      </c>
+      <c r="H25" s="23">
+        <v>0</v>
+      </c>
+      <c r="I25" s="24">
+        <v>-1</v>
+      </c>
+      <c r="J25" s="20">
+        <f>$G$3+G25+$H$3+H25+$I$3+I25</f>
+        <v>14</v>
+      </c>
+      <c r="L25" t="s">
         <v>27</v>
       </c>
-      <c r="M18">
-        <f>IF(J18=15,1,0) + IF(J19=15,1,0) + IF(J20=15,1,0)+ IF(J21=15,1,0)+ IF(I21=15,1,0) + IF(H21=15,1,0) + IF(G21=15,1,0) + IF(F21=15,1,0)</f>
+      <c r="M25">
+        <f>IF(J25=15,1,0) + IF(J26=15,1,0) + IF(J27=15,1,0)+ IF(J28=15,1,0)+ IF(I28=15,1,0) + IF(H28=15,1,0) + IF(G28=15,1,0) + IF(F28=15,1,0)</f>
         <v>5</v>
       </c>
-      <c r="O18" s="20"/>
-      <c r="P18" s="22">
-        <v>2</v>
-      </c>
-      <c r="Q18" s="23">
-        <v>1</v>
-      </c>
-      <c r="R18" s="24">
-        <v>0</v>
-      </c>
-      <c r="S18" s="20">
-        <f>$G$3+P18+$H$3+Q18+$I$3+R18</f>
-        <v>15</v>
-      </c>
-      <c r="U18" t="s">
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F26" s="20"/>
+      <c r="G26" s="25">
+        <v>0</v>
+      </c>
+      <c r="H26" s="26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="27">
+        <v>1</v>
+      </c>
+      <c r="J26" s="20">
+        <f>$G$4+G26+$H$4+H26+$I$4+I26</f>
+        <v>15</v>
+      </c>
+      <c r="L26" t="s">
+        <v>21</v>
+      </c>
+      <c r="M26">
+        <f>8-M25</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="20"/>
+      <c r="G27" s="28">
+        <v>0</v>
+      </c>
+      <c r="H27" s="29">
+        <v>3</v>
+      </c>
+      <c r="I27" s="30">
+        <v>0</v>
+      </c>
+      <c r="J27" s="20">
+        <f>$G$5+G27+$H$5+H27+$I$5+I27</f>
+        <v>15</v>
+      </c>
+      <c r="L27" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27">
+        <f>ABS(G25)+ABS(H25)+ABS(I25)+ABS(G26)+ABS(H26)+ABS(I26)+ABS(G27)+ABS(H27)+ABS(I27)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F28" s="20">
+        <f>G27+H26+I25+$G$5+$H$4+$I$3</f>
+        <v>14</v>
+      </c>
+      <c r="G28" s="20">
+        <f>$G$3+G25+$G$4+G26+$G$5+G27</f>
+        <v>15</v>
+      </c>
+      <c r="H28" s="20">
+        <f>H27+$H$5+H26+$H$4+H25+$H$3</f>
+        <v>15</v>
+      </c>
+      <c r="I28" s="20">
+        <f>I27+$I$5+I26+$I$4+I25+$I$3</f>
+        <v>14</v>
+      </c>
+      <c r="J28" s="20">
+        <f>$G$3+G25+$H$4+H26+$I$5+I27</f>
+        <v>15</v>
+      </c>
+      <c r="L28" t="s">
+        <v>28</v>
+      </c>
+      <c r="M28">
+        <f>((M26)+1)^2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29">
+        <f>(M26+M27)*M28</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="33"/>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F33" s="20"/>
+      <c r="G33" s="22">
+        <v>1</v>
+      </c>
+      <c r="H33" s="23">
+        <v>0</v>
+      </c>
+      <c r="I33" s="24">
+        <v>-1</v>
+      </c>
+      <c r="J33" s="20">
+        <f>$G$3+G33+$H$3+H33+$I$3+I33</f>
+        <v>12</v>
+      </c>
+      <c r="L33" t="s">
         <v>27</v>
       </c>
-      <c r="V18">
-        <f>IF(S18=15,1,0) + IF(S19=15,1,0) + IF(S20=15,1,0)+ IF(S21=15,1,0)+ IF(R21=15,1,0) + IF(Q21=15,1,0) + IF(P21=15,1,0) + IF(O21=15,1,0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="E19" s="21"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="25">
-        <v>0</v>
-      </c>
-      <c r="H19" s="26">
-        <v>0</v>
-      </c>
-      <c r="I19" s="27">
-        <v>1</v>
-      </c>
-      <c r="J19" s="20">
-        <f>$G$4+G19+$H$4+H19+$I$4+I19</f>
-        <v>15</v>
-      </c>
-      <c r="L19" t="s">
-        <v>21</v>
-      </c>
-      <c r="M19">
-        <f>8-M18</f>
-        <v>3</v>
-      </c>
-      <c r="O19" s="20"/>
-      <c r="P19" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="26">
-        <v>0</v>
-      </c>
-      <c r="R19" s="27">
-        <v>0</v>
-      </c>
-      <c r="S19" s="20">
-        <f>$G$4+P19+$H$4+Q19+$I$4+R19</f>
-        <v>15</v>
-      </c>
-      <c r="U19" t="s">
-        <v>21</v>
-      </c>
-      <c r="V19">
-        <f>8-V18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="20"/>
-      <c r="G20" s="28">
-        <v>0</v>
-      </c>
-      <c r="H20" s="29">
-        <v>3</v>
-      </c>
-      <c r="I20" s="30">
-        <v>0</v>
-      </c>
-      <c r="J20" s="20">
-        <f>$G$5+G20+$H$5+H20+$I$5+I20</f>
-        <v>15</v>
-      </c>
-      <c r="L20" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20">
-        <f>ABS(G18)+ABS(H18)+ABS(I18)+ABS(G19)+ABS(H19)+ABS(I19)+ABS(G20)+ABS(H20)+ABS(I20)</f>
-        <v>8</v>
-      </c>
-      <c r="O20" s="20"/>
-      <c r="P20" s="28">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="29">
-        <v>2</v>
-      </c>
-      <c r="R20" s="30">
-        <v>1</v>
-      </c>
-      <c r="S20" s="20">
-        <f>$G$5+P20+$H$5+Q20+$I$5+R20</f>
-        <v>15</v>
-      </c>
-      <c r="U20" t="s">
-        <v>22</v>
-      </c>
-      <c r="V20">
-        <f>ABS(P18)+ABS(Q18)+ABS(R18)+ABS(P19)+ABS(Q19)+ABS(R19)+ABS(P20)+ABS(Q20)+ABS(R20)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="20">
-        <f>G20+H19+I18+$G$5+$H$4+$I$3</f>
-        <v>16</v>
-      </c>
-      <c r="G21" s="20">
-        <f>$G$3+G18+$G$4+G19+$G$5+G20</f>
-        <v>15</v>
-      </c>
-      <c r="H21" s="20">
-        <f>H20+$H$5+H19+$H$4+H18+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="I21" s="20">
-        <f>I20+$I$5+I19+$I$4+I18+$I$3</f>
-        <v>16</v>
-      </c>
-      <c r="J21" s="20">
-        <f>$G$3+G18+$H$4+H19+$I$5+I20</f>
-        <v>15</v>
-      </c>
-      <c r="L21" t="s">
-        <v>28</v>
-      </c>
-      <c r="M21">
-        <f>((M19)+1)^2</f>
-        <v>16</v>
-      </c>
-      <c r="O21" s="20">
-        <f>P20+Q19+R18+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="P21" s="20">
-        <f>$G$3+P18+$G$4+P19+$G$5+P20</f>
-        <v>15</v>
-      </c>
-      <c r="Q21" s="20">
-        <f>Q20+$H$5+Q19+$H$4+Q18+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="R21" s="20">
-        <f>R20+$I$5+R19+$I$4+R18+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="S21" s="20">
-        <f>$G$3+P18+$H$4+Q19+$I$5+R20</f>
-        <v>15</v>
-      </c>
-      <c r="U21" t="s">
-        <v>28</v>
-      </c>
-      <c r="V21">
-        <f>((V19)+1)^2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="L22" t="s">
-        <v>30</v>
-      </c>
-      <c r="M22">
-        <f>(M19+M20)*M21</f>
-        <v>176</v>
-      </c>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="U22" t="s">
-        <v>30</v>
-      </c>
-      <c r="V22">
-        <f>(V19+V20)*V21</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L25" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M25" s="33"/>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F26" s="20"/>
-      <c r="G26" s="22">
-        <v>3</v>
-      </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="24">
-        <v>-1</v>
-      </c>
-      <c r="J26" s="20">
-        <f>$G$3+G26+$H$3+H26+$I$3+I26</f>
-        <v>14</v>
-      </c>
-      <c r="L26" t="s">
-        <v>27</v>
-      </c>
-      <c r="M26">
-        <f>IF(J26=15,1,0) + IF(J27=15,1,0) + IF(J28=15,1,0)+ IF(J29=15,1,0)+ IF(I29=15,1,0) + IF(H29=15,1,0) + IF(G29=15,1,0) + IF(F29=15,1,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F27" s="20"/>
-      <c r="G27" s="25">
-        <v>0</v>
-      </c>
-      <c r="H27" s="26">
-        <v>0</v>
-      </c>
-      <c r="I27" s="27">
-        <v>1</v>
-      </c>
-      <c r="J27" s="20">
-        <f>$G$4+G27+$H$4+H27+$I$4+I27</f>
-        <v>15</v>
-      </c>
-      <c r="L27" t="s">
-        <v>21</v>
-      </c>
-      <c r="M27">
-        <f>8-M26</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="20"/>
-      <c r="G28" s="28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="29">
-        <v>3</v>
-      </c>
-      <c r="I28" s="30">
-        <v>0</v>
-      </c>
-      <c r="J28" s="20">
-        <f>$G$5+G28+$H$5+H28+$I$5+I28</f>
-        <v>15</v>
-      </c>
-      <c r="L28" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28">
-        <f>ABS(G26)+ABS(H26)+ABS(I26)+ABS(G27)+ABS(H27)+ABS(I27)+ABS(G28)+ABS(H28)+ABS(I28)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="F29" s="20">
-        <f>G28+H27+I26+$G$5+$H$4+$I$3</f>
-        <v>14</v>
-      </c>
-      <c r="G29" s="20">
-        <f>$G$3+G26+$G$4+G27+$G$5+G28</f>
-        <v>15</v>
-      </c>
-      <c r="H29" s="20">
-        <f>H28+$H$5+H27+$H$4+H26+$H$3</f>
-        <v>15</v>
-      </c>
-      <c r="I29" s="20">
-        <f>I28+$I$5+I27+$I$4+I26+$I$3</f>
-        <v>14</v>
-      </c>
-      <c r="J29" s="20">
-        <f>$G$3+G26+$H$4+H27+$I$5+I28</f>
-        <v>15</v>
-      </c>
-      <c r="L29" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29">
-        <f>((M27)+1)^2</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="L30" t="s">
-        <v>30</v>
-      </c>
-      <c r="M30">
-        <f>(M27+M28)*M29</f>
-        <v>176</v>
-      </c>
-    </row>
-    <row r="33" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L33" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M33" s="33"/>
+      <c r="M33">
+        <f>IF(J33=15,1,0) + IF(J34=15,1,0) + IF(J35=15,1,0)+ IF(J36=15,1,0)+ IF(I36=15,1,0) + IF(H36=15,1,0) + IF(G36=15,1,0) + IF(F36=15,1,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F34" s="20"/>
-      <c r="G34" s="22">
-        <v>1</v>
-      </c>
-      <c r="H34" s="23">
-        <v>0</v>
-      </c>
-      <c r="I34" s="24">
-        <v>-1</v>
+      <c r="G34" s="25">
+        <v>1</v>
+      </c>
+      <c r="H34" s="26">
+        <v>0</v>
+      </c>
+      <c r="I34" s="27">
+        <v>1</v>
       </c>
       <c r="J34" s="20">
-        <f>$G$3+G34+$H$3+H34+$I$3+I34</f>
+        <f>$G$4+G34+$H$4+H34+$I$4+I34</f>
+        <v>16</v>
+      </c>
+      <c r="L34" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34">
+        <f>8-M33</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="20"/>
+      <c r="G35" s="28">
+        <v>0</v>
+      </c>
+      <c r="H35" s="29">
+        <v>1</v>
+      </c>
+      <c r="I35" s="30">
+        <v>2</v>
+      </c>
+      <c r="J35" s="20">
+        <f>$G$5+G35+$H$5+H35+$I$5+I35</f>
+        <v>15</v>
+      </c>
+      <c r="L35" t="s">
+        <v>22</v>
+      </c>
+      <c r="M35">
+        <f>ABS(G33)+ABS(H33)+ABS(I33)+ABS(G34)+ABS(H34)+ABS(I34)+ABS(G35)+ABS(H35)+ABS(I35)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F36" s="20">
+        <f>G35+H34+I33+$G$5+$H$4+$I$3</f>
+        <v>14</v>
+      </c>
+      <c r="G36" s="20">
+        <f>$G$3+G33+$G$4+G34+$G$5+G35</f>
+        <v>14</v>
+      </c>
+      <c r="H36" s="20">
+        <f>H35+$H$5+H34+$H$4+H33+$H$3</f>
+        <v>13</v>
+      </c>
+      <c r="I36" s="20">
+        <f>I35+$I$5+I34+$I$4+I33+$I$3</f>
+        <v>16</v>
+      </c>
+      <c r="J36" s="20">
+        <f>$G$3+G33+$H$4+H34+$I$5+I35</f>
+        <v>15</v>
+      </c>
+      <c r="L36" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36">
+        <f>((M34)+1)^2</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>30</v>
+      </c>
+      <c r="M37">
+        <f>(M34+M35)*M36</f>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="40" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L40" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M40" s="33"/>
+    </row>
+    <row r="41" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F41" s="20"/>
+      <c r="G41" s="22">
+        <v>0</v>
+      </c>
+      <c r="H41" s="23">
+        <v>0</v>
+      </c>
+      <c r="I41" s="24">
+        <v>0</v>
+      </c>
+      <c r="J41" s="20">
+        <f>$G$3+G41+$H$3+H41+$I$3+I41</f>
         <v>12</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L41" t="s">
         <v>27</v>
       </c>
-      <c r="M34">
-        <f>IF(J34=15,1,0) + IF(J35=15,1,0) + IF(J36=15,1,0)+ IF(J37=15,1,0)+ IF(I37=15,1,0) + IF(H37=15,1,0) + IF(G37=15,1,0) + IF(F37=15,1,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F35" s="20"/>
-      <c r="G35" s="25">
-        <v>1</v>
-      </c>
-      <c r="H35" s="26">
-        <v>0</v>
-      </c>
-      <c r="I35" s="27">
-        <v>1</v>
-      </c>
-      <c r="J35" s="20">
-        <f>$G$4+G35+$H$4+H35+$I$4+I35</f>
-        <v>16</v>
-      </c>
-      <c r="L35" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35">
-        <f>8-M34</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="20"/>
-      <c r="G36" s="28">
-        <v>0</v>
-      </c>
-      <c r="H36" s="29">
-        <v>1</v>
-      </c>
-      <c r="I36" s="30">
-        <v>2</v>
-      </c>
-      <c r="J36" s="20">
-        <f>$G$5+G36+$H$5+H36+$I$5+I36</f>
-        <v>15</v>
-      </c>
-      <c r="L36" t="s">
-        <v>22</v>
-      </c>
-      <c r="M36">
-        <f>ABS(G34)+ABS(H34)+ABS(I34)+ABS(G35)+ABS(H35)+ABS(I35)+ABS(G36)+ABS(H36)+ABS(I36)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F37" s="20">
-        <f>G36+H35+I34+$G$5+$H$4+$I$3</f>
-        <v>14</v>
-      </c>
-      <c r="G37" s="20">
-        <f>$G$3+G34+$G$4+G35+$G$5+G36</f>
-        <v>14</v>
-      </c>
-      <c r="H37" s="20">
-        <f>H36+$H$5+H35+$H$4+H34+$H$3</f>
-        <v>13</v>
-      </c>
-      <c r="I37" s="20">
-        <f>I36+$I$5+I35+$I$4+I34+$I$3</f>
-        <v>16</v>
-      </c>
-      <c r="J37" s="20">
-        <f>$G$3+G34+$H$4+H35+$I$5+I36</f>
-        <v>15</v>
-      </c>
-      <c r="L37" t="s">
-        <v>28</v>
-      </c>
-      <c r="M37">
-        <f>((M35)+1)^2</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L38" t="s">
-        <v>30</v>
-      </c>
-      <c r="M38">
-        <f>(M35+M36)*M37</f>
-        <v>637</v>
-      </c>
-    </row>
-    <row r="41" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L41" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M41" s="33"/>
+      <c r="M41">
+        <f>IF(J41=15,1,0) + IF(J42=15,1,0) + IF(J43=15,1,0)+ IF(J44=15,1,0)+ IF(I44=15,1,0) + IF(H44=15,1,0) + IF(G44=15,1,0) + IF(F44=15,1,0)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="42" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F42" s="20"/>
-      <c r="G42" s="22">
-        <v>0</v>
-      </c>
-      <c r="H42" s="23">
-        <v>0</v>
-      </c>
-      <c r="I42" s="24">
+      <c r="G42" s="25">
+        <v>1</v>
+      </c>
+      <c r="H42" s="26">
+        <v>0</v>
+      </c>
+      <c r="I42" s="27">
         <v>0</v>
       </c>
       <c r="J42" s="20">
-        <f>$G$3+G42+$H$3+H42+$I$3+I42</f>
+        <f>$G$4+G42+$H$4+H42+$I$4+I42</f>
+        <v>15</v>
+      </c>
+      <c r="L42" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42">
+        <f>8-M41</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F43" s="20"/>
+      <c r="G43" s="28">
+        <v>0</v>
+      </c>
+      <c r="H43" s="29">
+        <v>0</v>
+      </c>
+      <c r="I43" s="30">
+        <v>0</v>
+      </c>
+      <c r="J43" s="20">
+        <f>$G$5+G43+$H$5+H43+$I$5+I43</f>
         <v>12</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L43" t="s">
+        <v>22</v>
+      </c>
+      <c r="M43">
+        <f>ABS(G41)+ABS(H41)+ABS(I41)+ABS(G42)+ABS(H42)+ABS(I42)+ABS(G43)+ABS(H43)+ABS(I43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F44" s="20">
+        <f>G43+H42+I41+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="G44" s="20">
+        <f>$G$3+G41+$G$4+G42+$G$5+G43</f>
+        <v>13</v>
+      </c>
+      <c r="H44" s="20">
+        <f>H43+$H$5+H42+$H$4+H41+$H$3</f>
+        <v>12</v>
+      </c>
+      <c r="I44" s="20">
+        <f>I43+$I$5+I42+$I$4+I41+$I$3</f>
+        <v>14</v>
+      </c>
+      <c r="J44" s="20">
+        <f>$G$3+G41+$H$4+H42+$I$5+I43</f>
+        <v>12</v>
+      </c>
+      <c r="L44" t="s">
+        <v>28</v>
+      </c>
+      <c r="M44">
+        <f>((M42)+1)^2</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="L45" t="s">
+        <v>30</v>
+      </c>
+      <c r="M45">
+        <f>(M42+M43)*M44</f>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L47" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="M47" s="33"/>
+    </row>
+    <row r="48" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F48" s="20"/>
+      <c r="G48" s="22">
+        <v>0</v>
+      </c>
+      <c r="H48" s="23">
+        <v>0</v>
+      </c>
+      <c r="I48" s="24">
+        <v>0</v>
+      </c>
+      <c r="J48" s="20">
+        <f>$G$3+G48+$H$3+H48+$I$3+I48</f>
+        <v>12</v>
+      </c>
+      <c r="L48" t="s">
         <v>27</v>
       </c>
-      <c r="M42">
-        <f>IF(J42=15,1,0) + IF(J43=15,1,0) + IF(J44=15,1,0)+ IF(J45=15,1,0)+ IF(I45=15,1,0) + IF(H45=15,1,0) + IF(G45=15,1,0) + IF(F45=15,1,0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F43" s="20"/>
-      <c r="G43" s="25">
-        <v>1</v>
-      </c>
-      <c r="H43" s="26">
-        <v>0</v>
-      </c>
-      <c r="I43" s="27">
-        <v>0</v>
-      </c>
-      <c r="J43" s="20">
-        <f>$G$4+G43+$H$4+H43+$I$4+I43</f>
-        <v>15</v>
-      </c>
-      <c r="L43" t="s">
-        <v>21</v>
-      </c>
-      <c r="M43">
-        <f>8-M42</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F44" s="20"/>
-      <c r="G44" s="28">
-        <v>0</v>
-      </c>
-      <c r="H44" s="29">
-        <v>0</v>
-      </c>
-      <c r="I44" s="30">
-        <v>0</v>
-      </c>
-      <c r="J44" s="20">
-        <f>$G$5+G44+$H$5+H44+$I$5+I44</f>
-        <v>12</v>
-      </c>
-      <c r="L44" t="s">
-        <v>22</v>
-      </c>
-      <c r="M44">
-        <f>ABS(G42)+ABS(H42)+ABS(I42)+ABS(G43)+ABS(H43)+ABS(I43)+ABS(G44)+ABS(H44)+ABS(I44)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F45" s="20">
-        <f>G44+H43+I42+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="G45" s="20">
-        <f>$G$3+G42+$G$4+G43+$G$5+G44</f>
-        <v>13</v>
-      </c>
-      <c r="H45" s="20">
-        <f>H44+$H$5+H43+$H$4+H42+$H$3</f>
-        <v>12</v>
-      </c>
-      <c r="I45" s="20">
-        <f>I44+$I$5+I43+$I$4+I42+$I$3</f>
-        <v>14</v>
-      </c>
-      <c r="J45" s="20">
-        <f>$G$3+G42+$H$4+H43+$I$5+I44</f>
-        <v>12</v>
-      </c>
-      <c r="L45" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45">
-        <f>((M43)+1)^2</f>
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L46" t="s">
-        <v>30</v>
-      </c>
-      <c r="M46">
-        <f>(M43+M44)*M45</f>
-        <v>343</v>
-      </c>
-    </row>
-    <row r="48" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L48" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="M48" s="33"/>
+      <c r="M48">
+        <f>IF(J48=15,1,0) + IF(J49=15,1,0) + IF(J50=15,1,0)+ IF(J51=15,1,0)+ IF(I51=15,1,0) + IF(H51=15,1,0) + IF(G51=15,1,0) + IF(F51=15,1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F49" s="20"/>
-      <c r="G49" s="22">
-        <v>0</v>
-      </c>
-      <c r="H49" s="23">
-        <v>0</v>
-      </c>
-      <c r="I49" s="24">
+      <c r="G49" s="25">
+        <v>0</v>
+      </c>
+      <c r="H49" s="26">
+        <v>0</v>
+      </c>
+      <c r="I49" s="27">
         <v>0</v>
       </c>
       <c r="J49" s="20">
-        <f>$G$3+G49+$H$3+H49+$I$3+I49</f>
+        <f>$G$4+G49+$H$4+H49+$I$4+I49</f>
+        <v>14</v>
+      </c>
+      <c r="L49" t="s">
+        <v>21</v>
+      </c>
+      <c r="M49">
+        <f>8-M48</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F50" s="20"/>
+      <c r="G50" s="28">
+        <v>0</v>
+      </c>
+      <c r="H50" s="29">
+        <v>0</v>
+      </c>
+      <c r="I50" s="30">
+        <v>0</v>
+      </c>
+      <c r="J50" s="20">
+        <f>$G$5+G50+$H$5+H50+$I$5+I50</f>
         <v>12</v>
       </c>
-      <c r="L49" t="s">
-        <v>27</v>
-      </c>
-      <c r="M49">
-        <f>IF(J49=15,1,0) + IF(J50=15,1,0) + IF(J51=15,1,0)+ IF(J52=15,1,0)+ IF(I52=15,1,0) + IF(H52=15,1,0) + IF(G52=15,1,0) + IF(F52=15,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F50" s="20"/>
-      <c r="G50" s="25">
-        <v>0</v>
-      </c>
-      <c r="H50" s="26">
-        <v>0</v>
-      </c>
-      <c r="I50" s="27">
-        <v>0</v>
-      </c>
-      <c r="J50" s="20">
-        <f>$G$4+G50+$H$4+H50+$I$4+I50</f>
+      <c r="L50" t="s">
+        <v>22</v>
+      </c>
+      <c r="M50">
+        <f>ABS(G48)+ABS(H48)+ABS(I48)+ABS(G49)+ABS(H49)+ABS(I49)+ABS(G50)+ABS(H50)+ABS(I50)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F51" s="20">
+        <f>G50+H49+I48+$G$5+$H$4+$I$3</f>
+        <v>15</v>
+      </c>
+      <c r="G51" s="20">
+        <f>$G$3+G48+$G$4+G49+$G$5+G50</f>
+        <v>12</v>
+      </c>
+      <c r="H51" s="20">
+        <f>H50+$H$5+H49+$H$4+H48+$H$3</f>
+        <v>12</v>
+      </c>
+      <c r="I51" s="20">
+        <f>I50+$I$5+I49+$I$4+I48+$I$3</f>
         <v>14</v>
       </c>
-      <c r="L50" t="s">
-        <v>21</v>
-      </c>
-      <c r="M50">
-        <f>8-M49</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="6:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F51" s="20"/>
-      <c r="G51" s="28">
-        <v>0</v>
-      </c>
-      <c r="H51" s="29">
-        <v>0</v>
-      </c>
-      <c r="I51" s="30">
-        <v>0</v>
-      </c>
       <c r="J51" s="20">
-        <f>$G$5+G51+$H$5+H51+$I$5+I51</f>
+        <f>$G$3+G48+$H$4+H49+$I$5+I50</f>
         <v>12</v>
       </c>
       <c r="L51" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M51">
-        <f>ABS(G49)+ABS(H49)+ABS(I49)+ABS(G50)+ABS(H50)+ABS(I50)+ABS(G51)+ABS(H51)+ABS(I51)</f>
-        <v>0</v>
+        <f>((M49)+1)^2</f>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F52" s="20">
-        <f>G51+H50+I49+$G$5+$H$4+$I$3</f>
-        <v>15</v>
-      </c>
-      <c r="G52" s="20">
-        <f>$G$3+G49+$G$4+G50+$G$5+G51</f>
-        <v>12</v>
-      </c>
-      <c r="H52" s="20">
-        <f>H51+$H$5+H50+$H$4+H49+$H$3</f>
-        <v>12</v>
-      </c>
-      <c r="I52" s="20">
-        <f>I51+$I$5+I50+$I$4+I49+$I$3</f>
-        <v>14</v>
-      </c>
-      <c r="J52" s="20">
-        <f>$G$3+G49+$H$4+H50+$I$5+I51</f>
-        <v>12</v>
-      </c>
       <c r="L52" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M52">
-        <f>((M50)+1)^2</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="53" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="L53" t="s">
-        <v>30</v>
-      </c>
-      <c r="M53">
-        <f>(M50+M51)*M52</f>
+        <f>(M49+M50)*M51</f>
         <v>448</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="AD9:AE9"/>
-    <mergeCell ref="U17:V17"/>
+  <mergeCells count="8">
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="U8:V8"/>
     <mergeCell ref="L2:M2"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="L40:M40"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="J3:J7 F6:I7">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
-      <formula>15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J10:J13 F13:I13">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
-      <formula>15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J18:J21 F21:I21">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J26:J29 F29:I29">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
-      <formula>15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J34:J37 F37:I37">
+  <conditionalFormatting sqref="J3:J6 F6:I6">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J42:J45 F45:I45">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="J9:J12 F12:I12">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J49:J52 F52:I52">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+  <conditionalFormatting sqref="J17:J20 F20:I20">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10:S13 O13:R13">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+  <conditionalFormatting sqref="J25:J28 F28:I28">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB10:AB13 X13:AA13">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+  <conditionalFormatting sqref="J33:J36 F36:I36">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>15</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18:S21 O21:R21">
+  <conditionalFormatting sqref="J41:J44 F44:I44">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48:J51 F51:I51">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S9:S12 O12:R12">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>15</formula>
     </cfRule>

</xml_diff>